<commit_message>
Fix: added clg, dep in subjects bulk
</commit_message>
<xml_diff>
--- a/erp/xlformats/subjects-bulk-format.xlsx
+++ b/erp/xlformats/subjects-bulk-format.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26719"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18BCEBFF-2EB4-4884-89B7-C4325B91641F}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anish\Downloads\Bulk Upload CGC CMS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Subject Code</t>
   </si>
@@ -38,12 +42,18 @@
   <si>
     <t>Subject Sem (e.g 1,2,3)</t>
   </si>
+  <si>
+    <t>Department ID</t>
+  </si>
+  <si>
+    <t>College ID</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -396,20 +406,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.26953125" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -419,7 +432,12 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>